<commit_message>
Code Cleanup and UI Beautification
</commit_message>
<xml_diff>
--- a/Underwater_Robot_NFC/bin/Debug/NFC.xlsx
+++ b/Underwater_Robot_NFC/bin/Debug/NFC.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcreng\git\Underwater_Robot_NFC\Underwater_Robot_NFC\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cs\Underwater_Robot_NFC\Underwater_Robot_NFC\bin\Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,11 +16,11 @@
     <sheet name="Transactions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TransactionsAB1" hidden="1">Transactions!$A:$B</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TransactionsAB" hidden="1">Transactions!$A:$B</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="41" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +52,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TransactionsAB1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TransactionsAB"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Team ID</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Total Balance</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>B</t>
@@ -117,29 +114,23 @@
     <t>L</t>
   </si>
   <si>
-    <t>23:28:24 Tuesday, 13 February 2018</t>
+    <t>Cursor</t>
   </si>
   <si>
-    <t>23:30:25 Tuesday, 13 February 2018</t>
+    <t>Background Data</t>
   </si>
   <si>
-    <t>23:30:37 Tuesday, 13 February 2018</t>
+    <t>Do Not Remove</t>
   </si>
   <si>
-    <t>23:31:16 Tuesday, 13 February 2018</t>
-  </si>
-  <si>
-    <t>23:34:40 Tuesday, 13 February 2018</t>
-  </si>
-  <si>
-    <t>23:34:53 Tuesday, 13 February 2018</t>
+    <t>A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +146,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -191,6 +196,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -234,8 +243,997 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Team Summary'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Balance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Team Summary'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Team Summary'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3EF3-4D5A-8683-13EFDA7B2809}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1562797999"/>
+        <c:axId val="1506945311"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1562797999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1506945311"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1506945311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1562797999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8458C031-2ADD-4BAA-8B3C-86F76F65D89D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="mcreng" refreshedDate="43144.982576620372" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{F430BDD0-9B3B-45F5-843E-FBCCC13ED0B2}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Cheung" refreshedDate="43145.604087731481" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{F430BDD0-9B3B-45F5-843E-FBCCC13ED0B2}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[Range].[Team ID].[Team ID]" caption="Team ID" numFmtId="0" level="1">
@@ -315,8 +1313,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91369B4A-FBCC-436E-B728-993769758696}" name="TeamPivotTable" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team ID">
-  <location ref="H1:I13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91369B4A-FBCC-436E-B728-993769758696}" name="TeamPivotTable" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team ID">
+  <location ref="H2:I14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
       <items count="12">
@@ -423,8 +1421,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CF24BA7-0E11-49F4-901C-4EEEDD1D8CFE}" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C14" xr:uid="{364474B5-068B-4253-A823-34BD16D97649}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CF24BA7-0E11-49F4-901C-4EEEDD1D8CFE}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C13" xr:uid="{364474B5-068B-4253-A823-34BD16D97649}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{75B7E3C5-E7A5-446E-BD3A-E1195419EFEE}" name="Team ID"/>
     <tableColumn id="2" xr3:uid="{A2E3AECD-0BDB-4EA6-BD6B-D49EB0763DA7}" name="School Name"/>
@@ -736,7 +1734,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <f>VLOOKUP(A2, Transactions!H:I, 2, FALSE)</f>
@@ -774,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(A3, Transactions!H:I, 2, FALSE)</f>
@@ -786,7 +1784,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <f>VLOOKUP(A4, Transactions!H:I, 2, FALSE)</f>
@@ -798,7 +1796,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <f>VLOOKUP(A5, Transactions!H:I, 2, FALSE)</f>
@@ -810,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <f>VLOOKUP(A6, Transactions!H:I, 2, FALSE)</f>
@@ -822,11 +1820,11 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <f>VLOOKUP(A7, Transactions!H:I, 2, FALSE)</f>
-        <v>420</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -834,7 +1832,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f>VLOOKUP(A8, Transactions!H:I, 2, FALSE)</f>
@@ -846,7 +1844,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <f>VLOOKUP(A9, Transactions!H:I, 2, FALSE)</f>
@@ -858,7 +1856,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <f>VLOOKUP(A10, Transactions!H:I, 2, FALSE)</f>
@@ -870,7 +1868,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <f>VLOOKUP(A11, Transactions!H:I, 2, FALSE)</f>
@@ -882,7 +1880,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <f>VLOOKUP(A12, Transactions!H:I, 2, FALSE)</f>
@@ -894,7 +1892,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <f>VLOOKUP(A13, Transactions!H:I, 2, FALSE)</f>
@@ -903,63 +1901,65 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687601F0-8128-4057-8810-74FDD610C7C1}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.21875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -967,13 +1967,17 @@
         <v>500</v>
       </c>
       <c r="H3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M3" s="6"/>
+      <c r="N3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -981,13 +1985,16 @@
         <v>500</v>
       </c>
       <c r="H4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -995,13 +2002,14 @@
         <v>500</v>
       </c>
       <c r="H5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I5" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1009,13 +2017,14 @@
         <v>500</v>
       </c>
       <c r="H6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1023,13 +2032,14 @@
         <v>500</v>
       </c>
       <c r="H7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I7" s="5">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1037,13 +2047,14 @@
         <v>500</v>
       </c>
       <c r="H8" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I8" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1051,13 +2062,14 @@
         <v>500</v>
       </c>
       <c r="H9" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1065,13 +2077,14 @@
         <v>500</v>
       </c>
       <c r="H10" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1079,13 +2092,14 @@
         <v>500</v>
       </c>
       <c r="H11" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I11" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1093,13 +2107,14 @@
         <v>500</v>
       </c>
       <c r="H12" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1107,77 +2122,21 @@
         <v>500</v>
       </c>
       <c r="H13" s="4">
+        <v>11</v>
+      </c>
+      <c r="I13" s="5">
+        <v>500</v>
+      </c>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H14" s="4">
         <v>12</v>
       </c>
-      <c r="I13" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>-10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>-30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>-5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17">
-        <v>-15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>-10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>-10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
+      <c r="I14" s="5">
+        <v>500</v>
+      </c>
+      <c r="M14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>